<commit_message>
delete spaces, comments and the mnemonic switch is almost done.
</commit_message>
<xml_diff>
--- a/CPUinstructionSet.xlsx
+++ b/CPUinstructionSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aevdm\Documents\programming\myOwnCompUwUter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aevdm\Documents\CPUproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E4BF75-7B04-4B60-8A40-DC36FC0D8B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197F8EEE-40E4-46DC-AC3C-C3EBD2C1FF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{08A94811-42EB-448B-AF4E-53CB7896B196}"/>
+    <workbookView xWindow="13690" yWindow="0" windowWidth="6630" windowHeight="10170" xr2:uid="{08A94811-42EB-448B-AF4E-53CB7896B196}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -47,15 +47,9 @@
     <t>AND</t>
   </si>
   <si>
-    <t>OR</t>
-  </si>
-  <si>
     <t>XOR</t>
   </si>
   <si>
-    <t>INV A</t>
-  </si>
-  <si>
     <t>A - B</t>
   </si>
   <si>
@@ -71,48 +65,24 @@
     <t>! A</t>
   </si>
   <si>
-    <t>INV B</t>
-  </si>
-  <si>
     <t>!B</t>
   </si>
   <si>
-    <t>A&lt;&lt;B</t>
-  </si>
-  <si>
-    <t>A&gt;&gt;B</t>
-  </si>
-  <si>
     <t>&gt;&gt; A by B</t>
   </si>
   <si>
     <t>&lt;&lt; A by B</t>
   </si>
   <si>
-    <t>IS ODD</t>
-  </si>
-  <si>
     <t xml:space="preserve"> A % 2 ? 1 : 0;</t>
   </si>
   <si>
-    <t>MULT</t>
-  </si>
-  <si>
     <t>A++</t>
   </si>
   <si>
     <t>A--</t>
   </si>
   <si>
-    <t>INCR</t>
-  </si>
-  <si>
-    <t>DECR</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>passthrough</t>
   </si>
   <si>
@@ -158,9 +128,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>CNT</t>
-  </si>
-  <si>
     <t>mem to reg</t>
   </si>
   <si>
@@ -213,6 +180,39 @@
   </si>
   <si>
     <t>jump if equal</t>
+  </si>
+  <si>
+    <t>LBS</t>
+  </si>
+  <si>
+    <t>RBS</t>
+  </si>
+  <si>
+    <t>NVB</t>
+  </si>
+  <si>
+    <t>NVA</t>
+  </si>
+  <si>
+    <t>ODD</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>DCR</t>
+  </si>
+  <si>
+    <t>ORE</t>
+  </si>
+  <si>
+    <t>PSS</t>
+  </si>
+  <si>
+    <t>ECT</t>
+  </si>
+  <si>
+    <t>MLT</t>
   </si>
 </sst>
 </file>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F26DA1-D68E-4ECE-81D9-189A96A5137F}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -762,10 +762,10 @@
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="20" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J1">
         <v>6</v>
@@ -812,10 +812,10 @@
       <c r="F2" s="4"/>
       <c r="G2" s="8"/>
       <c r="H2" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
@@ -840,18 +840,18 @@
       <c r="F3" s="1"/>
       <c r="G3" s="8"/>
       <c r="H3" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="15"/>
       <c r="M3" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
@@ -872,18 +872,18 @@
       <c r="F4" s="4"/>
       <c r="G4" s="8"/>
       <c r="H4" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="15"/>
       <c r="M4" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
@@ -904,18 +904,18 @@
       <c r="F5" s="1"/>
       <c r="G5" s="8"/>
       <c r="H5" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="15"/>
       <c r="M5" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
@@ -936,18 +936,18 @@
       <c r="F6" s="4"/>
       <c r="G6" s="8"/>
       <c r="H6" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="18" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
@@ -1087,23 +1087,23 @@
       <c r="F12" s="4"/>
       <c r="G12" s="8"/>
       <c r="H12" s="6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="18" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="18" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="15"/>
@@ -1121,13 +1121,13 @@
       <c r="F13" s="1"/>
       <c r="G13" s="8"/>
       <c r="H13" s="6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -1151,13 +1151,13 @@
       <c r="F14" s="4"/>
       <c r="G14" s="8"/>
       <c r="H14" s="6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
@@ -1181,13 +1181,13 @@
       <c r="F15" s="1"/>
       <c r="G15" s="8"/>
       <c r="H15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -1197,7 +1197,7 @@
       <c r="P15" s="14"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
@@ -1213,13 +1213,13 @@
       <c r="F16" s="4"/>
       <c r="G16" s="8"/>
       <c r="H16" s="6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -1229,7 +1229,7 @@
       <c r="P16" s="14"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
@@ -1245,10 +1245,10 @@
       <c r="F17" s="1"/>
       <c r="G17" s="8"/>
       <c r="H17" s="6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
@@ -1273,10 +1273,10 @@
       <c r="F18" s="4"/>
       <c r="G18" s="8"/>
       <c r="H18" s="6" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
@@ -1304,20 +1304,20 @@
         <v>0</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
       <c r="M19" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
       <c r="P19" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q19" s="14"/>
       <c r="R19" s="15"/>
@@ -1338,20 +1338,20 @@
         <v>1</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="15"/>
       <c r="M20" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
       <c r="P20" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q20" s="14"/>
       <c r="R20" s="15"/>
@@ -1372,20 +1372,20 @@
         <v>2</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="15"/>
       <c r="M21" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
       <c r="P21" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q21" s="14"/>
       <c r="R21" s="15"/>
@@ -1403,23 +1403,23 @@
       <c r="F22" s="4"/>
       <c r="G22" s="8"/>
       <c r="H22" s="6" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K22" s="14"/>
       <c r="L22" s="15"/>
       <c r="M22" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
       <c r="P22" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q22" s="14"/>
       <c r="R22" s="15"/>
@@ -1437,23 +1437,23 @@
       <c r="F23" s="1"/>
       <c r="G23" s="8"/>
       <c r="H23" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="15"/>
       <c r="M23" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
       <c r="P23" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q23" s="14"/>
       <c r="R23" s="15"/>
@@ -1471,18 +1471,18 @@
       <c r="F24" s="4"/>
       <c r="G24" s="8"/>
       <c r="H24" s="6" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K24" s="14"/>
       <c r="L24" s="15"/>
       <c r="M24" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
@@ -1503,18 +1503,18 @@
       <c r="F25" s="1"/>
       <c r="G25" s="8"/>
       <c r="H25" s="6" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="15"/>
       <c r="M25" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
@@ -1535,23 +1535,23 @@
       <c r="F26" s="4"/>
       <c r="G26" s="8"/>
       <c r="H26" s="6" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="15"/>
       <c r="M26" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
       <c r="P26" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q26" s="14"/>
       <c r="R26" s="15"/>
@@ -1569,23 +1569,23 @@
       <c r="F27" s="1"/>
       <c r="G27" s="8"/>
       <c r="H27" s="6" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K27" s="14"/>
       <c r="L27" s="15"/>
       <c r="M27" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
       <c r="P27" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q27" s="14"/>
       <c r="R27" s="15"/>
@@ -1603,23 +1603,23 @@
       <c r="F28" s="4"/>
       <c r="G28" s="8"/>
       <c r="H28" s="6" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K28" s="14"/>
       <c r="L28" s="15"/>
       <c r="M28" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
       <c r="P28" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q28" s="14"/>
       <c r="R28" s="15"/>
@@ -1637,7 +1637,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="8"/>
       <c r="H29" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="16"/>
@@ -1663,23 +1663,23 @@
       <c r="F30" s="4"/>
       <c r="G30" s="8"/>
       <c r="H30" s="6" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="15"/>
       <c r="M30" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
       <c r="P30" s="14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q30" s="14"/>
       <c r="R30" s="15"/>
@@ -1697,18 +1697,18 @@
       <c r="F31" s="1"/>
       <c r="G31" s="8"/>
       <c r="H31" s="6" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="18" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N31" s="11"/>
       <c r="O31" s="13"/>
@@ -1729,18 +1729,18 @@
       <c r="F32" s="4"/>
       <c r="G32" s="8"/>
       <c r="H32" s="6" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="15"/>
       <c r="M32" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
@@ -1761,18 +1761,18 @@
       <c r="F33" s="1"/>
       <c r="G33" s="8"/>
       <c r="H33" s="6" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="K33" s="14"/>
       <c r="L33" s="15"/>
       <c r="M33" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>

</xml_diff>

<commit_message>
mnemonic input makes puts bin in outp file
</commit_message>
<xml_diff>
--- a/CPUinstructionSet.xlsx
+++ b/CPUinstructionSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aevdm\Documents\CPUproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197F8EEE-40E4-46DC-AC3C-C3EBD2C1FF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA920E7-A24B-4369-B63B-3F7527417B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13690" yWindow="0" windowWidth="6630" windowHeight="10170" xr2:uid="{08A94811-42EB-448B-AF4E-53CB7896B196}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{08A94811-42EB-448B-AF4E-53CB7896B196}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F26DA1-D68E-4ECE-81D9-189A96A5137F}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>